<commit_message>
adding fillers without danish letters
</commit_message>
<xml_diff>
--- a/fillers.xlsx
+++ b/fillers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/choosing_sentences/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/arithmetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="499" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FB07C56-EFD3-4F0D-804D-E990FC21CF8F}"/>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Adding math-prefix to fillers file
</commit_message>
<xml_diff>
--- a/fillers.xlsx
+++ b/fillers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/arithmetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="499" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FB07C56-EFD3-4F0D-804D-E990FC21CF8F}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F0DE82-CCC2-4F9F-AE10-4A0E9C436CA1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,18 +42,6 @@
     <t>sentence</t>
   </si>
   <si>
-    <t>addition</t>
-  </si>
-  <si>
-    <t>subtraction</t>
-  </si>
-  <si>
-    <t>multiplication</t>
-  </si>
-  <si>
-    <t>division</t>
-  </si>
-  <si>
     <t>67 + 30 =</t>
   </si>
   <si>
@@ -474,6 +462,18 @@
   </si>
   <si>
     <t>63 / 9 =</t>
+  </si>
+  <si>
+    <t>math_addition</t>
+  </si>
+  <si>
+    <t>math_subtraction</t>
+  </si>
+  <si>
+    <t>math_multiplication</t>
+  </si>
+  <si>
+    <t>math_division</t>
   </si>
 </sst>
 </file>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,34 +829,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -864,19 +864,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>45</v>
@@ -896,19 +896,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>64</v>
@@ -929,19 +929,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>97</v>
@@ -964,16 +964,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>46</v>
@@ -993,19 +993,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>26</v>
@@ -1025,19 +1025,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G7">
         <v>57</v>
@@ -1057,19 +1057,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <v>39</v>
@@ -1089,19 +1089,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G9">
         <v>19</v>
@@ -1121,19 +1121,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G10">
         <v>38</v>
@@ -1153,19 +1153,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G11">
         <v>31</v>
@@ -1185,19 +1185,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G12">
         <v>65</v>
@@ -1217,19 +1217,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G13">
         <v>21</v>
@@ -1249,19 +1249,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>46</v>
@@ -1281,19 +1281,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G15">
         <v>72</v>
@@ -1313,19 +1313,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G16">
         <v>79</v>
@@ -1345,19 +1345,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G17">
         <v>62</v>
@@ -1377,19 +1377,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G18">
         <v>29</v>
@@ -1409,19 +1409,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G19">
         <v>44</v>
@@ -1441,19 +1441,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G20">
         <v>81</v>
@@ -1473,19 +1473,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G21">
         <v>29</v>
@@ -1505,19 +1505,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G22">
         <v>46</v>
@@ -1537,19 +1537,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G23">
         <v>39</v>
@@ -1569,19 +1569,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G24">
         <v>55</v>
@@ -1601,19 +1601,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G25">
         <v>64</v>
@@ -1633,19 +1633,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G26">
         <v>86</v>
@@ -1665,19 +1665,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G27">
         <v>26</v>
@@ -1697,19 +1697,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G28">
         <v>19</v>

</xml_diff>